<commit_message>
added some stuff /n fixed bugs and improved get* funcs/
</commit_message>
<xml_diff>
--- a/compounds_db.xlsx
+++ b/compounds_db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\PythonProject2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\numMethInChem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD444DE2-688B-4F40-A7C0-D9C9E041ABBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1CB53C-FF08-4654-9361-5845565409D0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="555" yWindow="495" windowWidth="28245" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Formula</t>
   </si>
@@ -109,10 +109,13 @@
     <t>hidrogen</t>
   </si>
   <si>
-    <t>3,26*10^(-3)</t>
-  </si>
-  <si>
-    <t>0,502*10^5</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>N2O</t>
+  </si>
+  <si>
+    <t>nitrogen (II) oxide</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="A12:M17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -802,20 +805,90 @@
       <c r="F11">
         <v>27.28</v>
       </c>
-      <c r="G11" t="s">
-        <v>29</v>
+      <c r="G11">
+        <v>3.2599999999999999E-3</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" t="s">
-        <v>30</v>
+      <c r="I11">
+        <v>50200</v>
       </c>
       <c r="J11">
         <v>298</v>
       </c>
       <c r="K11">
         <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>91.3</v>
+      </c>
+      <c r="E12">
+        <v>210.64</v>
+      </c>
+      <c r="F12">
+        <v>29.6</v>
+      </c>
+      <c r="G12">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>-59000</v>
+      </c>
+      <c r="J12">
+        <v>298</v>
+      </c>
+      <c r="K12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>82</v>
+      </c>
+      <c r="E13">
+        <v>219.83</v>
+      </c>
+      <c r="F13">
+        <v>45.7</v>
+      </c>
+      <c r="G13">
+        <v>8.6E-3</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>-853000</v>
+      </c>
+      <c r="J13">
+        <v>298</v>
+      </c>
+      <c r="K13">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>